<commit_message>
opd summary report init
</commit_message>
<xml_diff>
--- a/storage/OPDSUMMARYREPORT_TEMPLATE.xlsx
+++ b/storage/OPDSUMMARYREPORT_TEMPLATE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\cesu\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B328D353-C2F4-4EA0-9E17-398ED787ED4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D699B29-8B42-4AB4-AFB9-DFEBC3F544F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +96,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -162,31 +170,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -472,7 +484,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,66 +493,66 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
       <c r="T1" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6" t="s">
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6" t="s">
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
       <c r="T2" s="9"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -604,7 +616,7 @@
       <c r="T3" s="9"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2">
@@ -661,47 +673,47 @@
       <c r="S4" s="2">
         <v>0</v>
       </c>
-      <c r="T4" s="7">
+      <c r="T4" s="6">
         <f>SUM(G5,M5,S5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="2">
         <f>SUM(B4:G4)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
       <c r="M5" s="2">
         <f>SUM(H4:M4)</f>
         <v>0</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
       <c r="S5" s="2">
         <f>SUM(N4:S4)</f>
         <v>0</v>
       </c>
-      <c r="T5" s="8"/>
+      <c r="T5" s="7"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -729,43 +741,46 @@
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="5">
+        <f>SUM(B7:S7)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:L5"/>
     <mergeCell ref="T4:T5"/>
     <mergeCell ref="N1:S1"/>
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="T1:T3"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="H5:L5"/>
     <mergeCell ref="N5:R5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>